<commit_message>
Cambios menores y fix de error.
</commit_message>
<xml_diff>
--- a/caso 2/caso2_excel.xlsx
+++ b/caso 2/caso2_excel.xlsx
@@ -551,10 +551,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R60"/>
+  <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26:S63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
@@ -1244,11 +1244,25 @@
           <t>C3</t>
         </is>
       </c>
-      <c r="N28" s="10" t="n"/>
+      <c r="N28" s="10" t="inlineStr">
+        <is>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>CF1</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>CF2</t>
+        </is>
+      </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" t="n">
-        <v>3407006.617647059</v>
+        <v>3376056.321621621</v>
       </c>
       <c r="E29" s="10" t="n">
         <v>1</v>
@@ -1257,7 +1271,7 @@
         <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>7058.823529411765</v>
+        <v>0</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
@@ -1265,12 +1279,21 @@
         </is>
       </c>
       <c r="J29" t="n">
-        <v>1400.000000000002</v>
+        <v>1399.999999999995</v>
       </c>
       <c r="K29" t="n">
         <v>0</v>
       </c>
       <c r="L29" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" t="n">
+        <v>1</v>
+      </c>
+      <c r="O29" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1290,13 +1313,22 @@
         </is>
       </c>
       <c r="J30" t="n">
-        <v>6099.999999999998</v>
+        <v>6100.000000000005</v>
       </c>
       <c r="K30" t="n">
         <v>6900</v>
       </c>
       <c r="L30" t="n">
         <v>5000</v>
+      </c>
+      <c r="N30" t="n">
+        <v>2</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="31" ht="12.75" customHeight="1">
@@ -1309,15 +1341,33 @@
       <c r="G31" t="n">
         <v>0</v>
       </c>
+      <c r="N31" t="n">
+        <v>3</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0</v>
+      </c>
+      <c r="P31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="E32" s="10" t="n">
         <v>4</v>
       </c>
       <c r="F32" s="10" t="n">
-        <v>1749.999999999999</v>
+        <v>1119.999999999998</v>
       </c>
       <c r="G32" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" t="n">
+        <v>4</v>
+      </c>
+      <c r="O32" t="n">
+        <v>9755.199999999983</v>
+      </c>
+      <c r="P32" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1329,7 +1379,16 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>0</v>
+        <v>4181.351351351354</v>
+      </c>
+      <c r="N33" t="n">
+        <v>5</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0</v>
+      </c>
+      <c r="P33" t="n">
+        <v>48921.81081081084</v>
       </c>
     </row>
     <row r="34" ht="12.75" customHeight="1">
@@ -1342,7 +1401,15 @@
       <c r="G34" t="n">
         <v>0</v>
       </c>
-      <c r="N34" s="10" t="n"/>
+      <c r="N34" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="O34" t="n">
+        <v>0</v>
+      </c>
+      <c r="P34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" ht="12.75" customHeight="1">
       <c r="E35" t="n">
@@ -1354,6 +1421,15 @@
       <c r="G35" t="n">
         <v>0</v>
       </c>
+      <c r="N35" t="n">
+        <v>7</v>
+      </c>
+      <c r="O35" t="n">
+        <v>0</v>
+      </c>
+      <c r="P35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" ht="12.75" customHeight="1">
       <c r="E36" t="n">
@@ -1363,10 +1439,39 @@
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>4750</v>
+      </c>
+      <c r="N36" t="n">
+        <v>8</v>
+      </c>
+      <c r="O36" t="n">
+        <v>0</v>
+      </c>
+      <c r="P36" t="n">
+        <v>20377.5</v>
       </c>
     </row>
     <row r="38" ht="12.75" customHeight="1">
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>S4</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
       <c r="I38" t="inlineStr">
         <is>
           <t>S5</t>
@@ -1404,6 +1509,20 @@
       </c>
     </row>
     <row r="39" ht="12.75" customHeight="1">
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>CF1</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>288119.9999999991</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0</v>
+      </c>
       <c r="I39" t="n">
         <v>1</v>
       </c>
@@ -1411,7 +1530,7 @@
         <v>0</v>
       </c>
       <c r="K39" t="n">
-        <v>86470.58823529411</v>
+        <v>0</v>
       </c>
       <c r="N39" t="inlineStr">
         <is>
@@ -1419,7 +1538,7 @@
         </is>
       </c>
       <c r="O39" t="n">
-        <v>288120.0000000004</v>
+        <v>20299.99999999993</v>
       </c>
       <c r="P39" t="n">
         <v>0</v>
@@ -1429,6 +1548,20 @@
       </c>
     </row>
     <row r="40" ht="12.75" customHeight="1">
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>CF2</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>973560.0000000007</v>
+      </c>
+      <c r="G40" t="n">
+        <v>1049490</v>
+      </c>
+      <c r="H40" t="n">
+        <v>708100</v>
+      </c>
       <c r="I40" t="n">
         <v>2</v>
       </c>
@@ -1444,13 +1577,13 @@
         </is>
       </c>
       <c r="O40" t="n">
-        <v>973559.9999999997</v>
+        <v>84790.00000000006</v>
       </c>
       <c r="P40" t="n">
-        <v>1049490</v>
+        <v>95910</v>
       </c>
       <c r="Q40" t="n">
-        <v>708100</v>
+        <v>69500</v>
       </c>
     </row>
     <row r="41" ht="12.75" customHeight="1">
@@ -1469,7 +1602,7 @@
         <v>4</v>
       </c>
       <c r="J42" t="n">
-        <v>15242.49999999999</v>
+        <v>447.9999999999992</v>
       </c>
       <c r="K42" t="n">
         <v>0</v>
@@ -1483,7 +1616,7 @@
         <v>0</v>
       </c>
       <c r="K43" t="n">
-        <v>0</v>
+        <v>2508.810810810812</v>
       </c>
     </row>
     <row r="44" ht="12.75" customHeight="1">
@@ -1516,7 +1649,7 @@
         <v>0</v>
       </c>
       <c r="K46" t="n">
-        <v>0</v>
+        <v>4275</v>
       </c>
     </row>
     <row r="48" ht="12.75" customHeight="1">
@@ -1562,12 +1695,17 @@
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>CF1</t>
+          <t>M1</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>CF2</t>
+          <t>M2</t>
+        </is>
+      </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>M3</t>
         </is>
       </c>
     </row>
@@ -1579,7 +1717,7 @@
         <v>0</v>
       </c>
       <c r="G49" t="n">
-        <v>14823.52941176471</v>
+        <v>0</v>
       </c>
       <c r="I49" t="inlineStr">
         <is>
@@ -1587,7 +1725,7 @@
         </is>
       </c>
       <c r="J49" t="n">
-        <v>20300.00000000003</v>
+        <v>308419.999999999</v>
       </c>
       <c r="K49" t="n">
         <v>0</v>
@@ -1595,14 +1733,19 @@
       <c r="L49" t="n">
         <v>0</v>
       </c>
-      <c r="N49" t="n">
-        <v>1</v>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>CF1</t>
+        </is>
       </c>
       <c r="O49" t="n">
         <v>0</v>
       </c>
       <c r="P49" t="n">
-        <v>101294.1176470588</v>
+        <v>1399.999999999997</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="50" ht="12.75" customHeight="1">
@@ -1621,22 +1764,27 @@
         </is>
       </c>
       <c r="J50" t="n">
-        <v>84789.99999999997</v>
+        <v>1058350.000000001</v>
       </c>
       <c r="K50" t="n">
-        <v>95910</v>
+        <v>1145400</v>
       </c>
       <c r="L50" t="n">
-        <v>69500</v>
-      </c>
-      <c r="N50" t="n">
-        <v>2</v>
+        <v>777600</v>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>CF2</t>
+        </is>
       </c>
       <c r="O50" t="n">
         <v>0</v>
       </c>
       <c r="P50" t="n">
-        <v>0</v>
+        <v>5162.162162162164</v>
+      </c>
+      <c r="Q50" t="n">
+        <v>12837.83783783784</v>
       </c>
     </row>
     <row r="51" ht="12.75" customHeight="1">
@@ -1649,33 +1797,15 @@
       <c r="G51" t="n">
         <v>0</v>
       </c>
-      <c r="N51" t="n">
-        <v>3</v>
-      </c>
-      <c r="O51" t="n">
-        <v>0</v>
-      </c>
-      <c r="P51" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="52" ht="12.75" customHeight="1">
       <c r="E52" t="n">
         <v>4</v>
       </c>
       <c r="F52" t="n">
-        <v>699.9999999999998</v>
+        <v>10203.19999999998</v>
       </c>
       <c r="G52" t="n">
-        <v>0</v>
-      </c>
-      <c r="N52" t="n">
-        <v>4</v>
-      </c>
-      <c r="O52" t="n">
-        <v>15942.49999999999</v>
-      </c>
-      <c r="P52" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1687,16 +1817,7 @@
         <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>0</v>
-      </c>
-      <c r="N53" t="n">
-        <v>5</v>
-      </c>
-      <c r="O53" t="n">
-        <v>0</v>
-      </c>
-      <c r="P53" t="n">
-        <v>0</v>
+        <v>51430.62162162165</v>
       </c>
     </row>
     <row r="54" ht="12.75" customHeight="1">
@@ -1709,15 +1830,6 @@
       <c r="G54" t="n">
         <v>0</v>
       </c>
-      <c r="N54" t="n">
-        <v>6</v>
-      </c>
-      <c r="O54" t="n">
-        <v>0</v>
-      </c>
-      <c r="P54" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="55" ht="12.75" customHeight="1">
       <c r="E55" t="n">
@@ -1729,15 +1841,6 @@
       <c r="G55" t="n">
         <v>0</v>
       </c>
-      <c r="N55" t="n">
-        <v>7</v>
-      </c>
-      <c r="O55" t="n">
-        <v>0</v>
-      </c>
-      <c r="P55" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="56" ht="12.75" customHeight="1">
       <c r="E56" t="n">
@@ -1747,120 +1850,12 @@
         <v>0</v>
       </c>
       <c r="G56" t="n">
-        <v>0</v>
-      </c>
-      <c r="N56" t="n">
-        <v>8</v>
-      </c>
-      <c r="O56" t="n">
-        <v>0</v>
-      </c>
-      <c r="P56" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" ht="12.75" customHeight="1">
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>S10</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>C2</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>C3</t>
-        </is>
-      </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>S11</t>
-        </is>
-      </c>
-      <c r="J58" t="inlineStr">
-        <is>
-          <t>M1</t>
-        </is>
-      </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>M2</t>
-        </is>
-      </c>
-      <c r="L58" t="inlineStr">
-        <is>
-          <t>M3</t>
-        </is>
-      </c>
-    </row>
-    <row r="59" ht="12.75" customHeight="1">
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>CF1</t>
-        </is>
-      </c>
-      <c r="F59" t="n">
-        <v>308420.0000000004</v>
-      </c>
-      <c r="G59" t="n">
-        <v>0</v>
-      </c>
-      <c r="H59" t="n">
-        <v>0</v>
-      </c>
-      <c r="I59" t="inlineStr">
-        <is>
-          <t>CF1</t>
-        </is>
-      </c>
-      <c r="J59" t="n">
-        <v>0</v>
-      </c>
-      <c r="K59" t="n">
-        <v>1400</v>
-      </c>
-      <c r="L59" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" ht="12.75" customHeight="1">
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>CF2</t>
-        </is>
-      </c>
-      <c r="F60" t="n">
-        <v>1058350</v>
-      </c>
-      <c r="G60" t="n">
-        <v>1145400</v>
-      </c>
-      <c r="H60" t="n">
-        <v>777600</v>
-      </c>
-      <c r="I60" t="inlineStr">
-        <is>
-          <t>CF2</t>
-        </is>
-      </c>
-      <c r="J60" t="n">
-        <v>18000</v>
-      </c>
-      <c r="K60" t="n">
-        <v>0</v>
-      </c>
-      <c r="L60" t="n">
-        <v>0</v>
-      </c>
-    </row>
+        <v>24652.5</v>
+      </c>
+    </row>
+    <row r="58" ht="12.75" customHeight="1"/>
+    <row r="59" ht="12.75" customHeight="1"/>
+    <row r="60" ht="12.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="N2:O2"/>

</xml_diff>